<commit_message>
import revised with new fields
</commit_message>
<xml_diff>
--- a/public/excel_samples/rider_invoice.xlsx
+++ b/public/excel_samples/rider_invoice.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Invoice Description comes here</t>
+  </si>
+  <si>
+    <t>Gaurantee</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD329"/>
+  <dimension ref="A1:AE329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +500,7 @@
     <col min="30" max="30" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -588,8 +591,11 @@
       <c r="AD1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45341</v>
       </c>
@@ -675,52 +681,52 @@
         <v>27</v>
       </c>
       <c r="AC2" s="1">
-        <v>44927</v>
+        <v>45292</v>
       </c>
       <c r="AD2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC13" s="1"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC15" s="1"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC16" s="1"/>
     </row>
     <row r="17" spans="29:29" x14ac:dyDescent="0.25">
@@ -1664,5 +1670,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
import invoice updated with sim and bike charges
</commit_message>
<xml_diff>
--- a/public/excel_samples/rider_invoice.xlsx
+++ b/public/excel_samples/rider_invoice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adnan_uae\erp_express\public\excel_samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perza\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Gaurantee</t>
+  </si>
+  <si>
+    <t>Bike &amp; Sim Charges</t>
+  </si>
+  <si>
+    <t>Jan-2024</t>
   </si>
 </sst>
 </file>
@@ -167,10 +173,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE329"/>
+  <dimension ref="A1:AF329"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +507,7 @@
     <col min="30" max="30" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -594,8 +601,11 @@
       <c r="AE1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45341</v>
       </c>
@@ -680,53 +690,56 @@
       <c r="AB2" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="1">
-        <v>45292</v>
+      <c r="AC2" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="AD2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC13" s="1"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC15" s="1"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AC16" s="1"/>
     </row>
     <row r="17" spans="29:29" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
rider invoice import updated with rta fine and fuel vouchers
</commit_message>
<xml_diff>
--- a/public/excel_samples/rider_invoice.xlsx
+++ b/public/excel_samples/rider_invoice.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="10470"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>Jan-2024</t>
+  </si>
+  <si>
+    <t>Fuel Charges</t>
+  </si>
+  <si>
+    <t>Fuel Narration</t>
+  </si>
+  <si>
+    <t>RTA charges</t>
+  </si>
+  <si>
+    <t>RTA Narration</t>
   </si>
 </sst>
 </file>
@@ -492,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF329"/>
+  <dimension ref="A1:AJ329"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+      <selection activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,9 +517,15 @@
     <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -604,8 +622,20 @@
       <c r="AF1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45341</v>
       </c>
@@ -700,46 +730,46 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC13" s="1"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC15" s="1"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AC16" s="1"/>
     </row>
     <row r="17" spans="29:29" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
rider invoice import and add edit and show with notes
</commit_message>
<xml_diff>
--- a/public/excel_samples/rider_invoice.xlsx
+++ b/public/excel_samples/rider_invoice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perza\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adnan_uae\erp_express\public\excel_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>RTA Narration</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ329"/>
+  <dimension ref="A1:AK329"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
       <selection activeCell="AK1" sqref="AK1"/>
@@ -525,7 +528,7 @@
     <col min="36" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -634,8 +637,11 @@
       <c r="AJ1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45341</v>
       </c>
@@ -730,46 +736,46 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC13" s="1"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC15" s="1"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AC16" s="1"/>
     </row>
     <row r="17" spans="29:29" x14ac:dyDescent="0.25">

</xml_diff>